<commit_message>
Firm v0.3 - actualizacion de config, control options, about
</commit_message>
<xml_diff>
--- a/Firmware/v0.3 Stable - Hard 0.0/LCD Layout - Firm v03.xlsx
+++ b/Firmware/v0.3 Stable - Hard 0.0/LCD Layout - Firm v03.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="764" uniqueCount="70">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="774" uniqueCount="73">
   <si>
     <t>01</t>
   </si>
@@ -195,9 +195,6 @@
     <t>F</t>
   </si>
   <si>
-    <t>w</t>
-  </si>
-  <si>
     <t>S</t>
   </si>
   <si>
@@ -207,12 +204,6 @@
     <t>A</t>
   </si>
   <si>
-    <t>&gt;</t>
-  </si>
-  <si>
-    <t>&lt;</t>
-  </si>
-  <si>
     <t>k</t>
   </si>
   <si>
@@ -226,6 +217,24 @@
   </si>
   <si>
     <t>=</t>
+  </si>
+  <si>
+    <t>b</t>
+  </si>
+  <si>
+    <t>&amp;</t>
+  </si>
+  <si>
+    <t>/</t>
+  </si>
+  <si>
+    <t>Y</t>
+  </si>
+  <si>
+    <t>j</t>
+  </si>
+  <si>
+    <t>7</t>
   </si>
 </sst>
 </file>
@@ -620,8 +629,8 @@
   <sheetPr codeName="Hoja1"/>
   <dimension ref="A1:AF71"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M75" sqref="M75"/>
+    <sheetView tabSelected="1" topLeftCell="A43" workbookViewId="0">
+      <selection activeCell="X54" sqref="X54"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -710,162 +719,141 @@
       <c r="A2" s="2" t="s">
         <v>53</v>
       </c>
-      <c r="B2" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>25</v>
-      </c>
       <c r="D2" s="1" t="s">
-        <v>29</v>
+        <v>38</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>22</v>
+        <v>39</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>30</v>
+        <v>40</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="H2" s="1" t="s">
-        <v>31</v>
+        <v>43</v>
       </c>
       <c r="I2" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="J2" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="M2" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="N2" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="J2" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="K2" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="L2" s="1" t="s">
+      <c r="O2" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="P2" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="Q2" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="R2" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="S2" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="T2" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="M2" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="N2" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="O2" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="P2" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="Q2" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="R2" s="1" t="s">
-        <v>37</v>
+      <c r="U2" s="1" t="s">
+        <v>19</v>
       </c>
     </row>
     <row r="3" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B3" s="1" t="s">
-        <v>38</v>
-      </c>
       <c r="C3" s="1" t="s">
-        <v>39</v>
+        <v>28</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>40</v>
+        <v>25</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>20</v>
+        <v>31</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>41</v>
+        <v>25</v>
       </c>
       <c r="H3" s="1" t="s">
-        <v>42</v>
+        <v>45</v>
       </c>
       <c r="J3" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="K3" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="L3" s="1" t="s">
-        <v>35</v>
+        <v>68</v>
       </c>
       <c r="M3" s="1" t="s">
-        <v>24</v>
+        <v>48</v>
       </c>
       <c r="N3" s="1" t="s">
-        <v>44</v>
+        <v>23</v>
       </c>
       <c r="O3" s="1" t="s">
         <v>45</v>
       </c>
       <c r="P3" s="1" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="Q3" s="1" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="R3" s="1" t="s">
-        <v>26</v>
+        <v>47</v>
       </c>
       <c r="S3" s="1" t="s">
-        <v>25</v>
+        <v>19</v>
       </c>
       <c r="T3" s="1" t="s">
-        <v>45</v>
+        <v>34</v>
       </c>
       <c r="U3" s="1" t="s">
-        <v>63</v>
+        <v>19</v>
       </c>
     </row>
     <row r="4" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>1</v>
       </c>
+      <c r="B4" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="F4" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="G4" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="H4" s="1" t="s">
+        <v>26</v>
+      </c>
       <c r="I4" s="1" t="s">
-        <v>58</v>
+        <v>26</v>
       </c>
       <c r="J4" s="1" t="s">
-        <v>32</v>
+        <v>25</v>
       </c>
       <c r="K4" s="1" t="s">
         <v>45</v>
-      </c>
-      <c r="L4" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="M4" s="1" t="s">
-        <v>59</v>
-      </c>
-      <c r="N4" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="O4" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="P4" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="Q4" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="R4" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="S4" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="T4" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="U4" s="1" t="s">
-        <v>19</v>
       </c>
     </row>
     <row r="5" spans="1:32" x14ac:dyDescent="0.25">
@@ -873,58 +861,64 @@
         <v>2</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>30</v>
+        <v>22</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>38</v>
+        <v>44</v>
       </c>
       <c r="D5" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="F5" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="E5" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="F5" s="1" t="s">
-        <v>19</v>
+      <c r="G5" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="H5" s="1" t="s">
+        <v>69</v>
       </c>
       <c r="I5" s="1" t="s">
-        <v>48</v>
+        <v>64</v>
       </c>
       <c r="J5" s="1" t="s">
-        <v>23</v>
+        <v>35</v>
       </c>
       <c r="K5" s="1" t="s">
-        <v>45</v>
+        <v>35</v>
       </c>
       <c r="L5" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="M5" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="N5" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="O5" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="P5" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="Q5" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="M5" s="1" t="s">
-        <v>59</v>
-      </c>
-      <c r="N5" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="O5" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="P5" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="Q5" s="1" t="s">
-        <v>27</v>
-      </c>
       <c r="R5" s="1" t="s">
-        <v>47</v>
+        <v>70</v>
       </c>
       <c r="S5" s="1" t="s">
-        <v>19</v>
+        <v>26</v>
       </c>
       <c r="T5" s="1" t="s">
-        <v>34</v>
+        <v>71</v>
       </c>
       <c r="U5" s="1" t="s">
-        <v>19</v>
+        <v>72</v>
       </c>
     </row>
     <row r="7" spans="1:32" s="3" customFormat="1" x14ac:dyDescent="0.25">
@@ -1515,7 +1509,7 @@
       </c>
       <c r="B22" s="5"/>
       <c r="C22" s="1" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="D22" s="1" t="s">
         <v>23</v>
@@ -2031,7 +2025,7 @@
         <v>55</v>
       </c>
       <c r="L39" s="1" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="M39" s="1" t="s">
         <v>23</v>
@@ -2304,6 +2298,25 @@
       <c r="A51" s="2" t="s">
         <v>0</v>
       </c>
+      <c r="C51" s="5"/>
+      <c r="D51" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="E51" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="F51" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="G51" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="H51" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="I51" s="1" t="s">
+        <v>55</v>
+      </c>
       <c r="M51" s="5"/>
       <c r="N51" s="1" t="s">
         <v>21</v>
@@ -2315,13 +2328,13 @@
         <v>24</v>
       </c>
       <c r="Q51" s="1" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="R51" s="1" t="s">
         <v>32</v>
       </c>
       <c r="S51" s="1" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
     </row>
     <row r="52" spans="1:21" x14ac:dyDescent="0.25">
@@ -2515,7 +2528,7 @@
         <v>51</v>
       </c>
       <c r="P56" s="1" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="Q56" s="1" t="s">
         <v>56</v>
@@ -2642,7 +2655,7 @@
         <v>2</v>
       </c>
       <c r="B59" s="6" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C59" s="1" t="s">
         <v>52</v>
@@ -2677,7 +2690,7 @@
       </c>
       <c r="O59" s="5"/>
       <c r="P59" s="6" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="Q59" s="1" t="s">
         <v>54</v>
@@ -2832,13 +2845,13 @@
         <v>19</v>
       </c>
       <c r="Q63" s="1" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="R63" s="1" t="s">
         <v>36</v>
       </c>
       <c r="S63" s="1" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="64" spans="1:21" x14ac:dyDescent="0.25">
@@ -2927,7 +2940,7 @@
       </c>
       <c r="P65" s="5"/>
       <c r="Q65" s="6" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="R65" s="1" t="s">
         <v>44</v>
@@ -3019,13 +3032,13 @@
         <v>24</v>
       </c>
       <c r="E68" s="1" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="F68" s="1" t="s">
         <v>32</v>
       </c>
       <c r="G68" s="1" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="H68" s="1" t="s">
         <v>27</v>
@@ -3043,18 +3056,23 @@
       <c r="G69" s="6"/>
       <c r="H69" s="6"/>
       <c r="I69" s="6"/>
-      <c r="J69" s="6"/>
-      <c r="K69" s="6"/>
-      <c r="L69" s="6"/>
-      <c r="M69" s="6"/>
-      <c r="N69" s="6"/>
       <c r="O69" s="6"/>
-      <c r="P69" s="6"/>
-      <c r="Q69" s="6"/>
-      <c r="R69" s="6"/>
-      <c r="S69" s="6"/>
-      <c r="T69" s="6"/>
-      <c r="U69" s="6"/>
+      <c r="P69" s="5"/>
+      <c r="Q69" s="6" t="s">
+        <v>61</v>
+      </c>
+      <c r="R69" s="6" t="s">
+        <v>67</v>
+      </c>
+      <c r="S69" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="T69" s="6" t="s">
+        <v>52</v>
+      </c>
+      <c r="U69" s="1" t="s">
+        <v>44</v>
+      </c>
     </row>
     <row r="70" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A70" s="2" t="s">
@@ -3070,7 +3088,7 @@
         <v>38</v>
       </c>
       <c r="F70" s="6" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="G70" s="6" t="s">
         <v>23</v>
@@ -3079,79 +3097,86 @@
         <v>29</v>
       </c>
       <c r="I70" s="6" t="s">
-        <v>65</v>
-      </c>
-      <c r="J70" s="6"/>
+        <v>62</v>
+      </c>
+      <c r="J70" s="6" t="s">
+        <v>49</v>
+      </c>
       <c r="K70" s="6" t="s">
-        <v>49</v>
+        <v>32</v>
       </c>
       <c r="L70" s="6" t="s">
-        <v>32</v>
+        <v>64</v>
       </c>
       <c r="M70" s="6" t="s">
-        <v>67</v>
+        <v>22</v>
       </c>
       <c r="N70" s="6" t="s">
-        <v>22</v>
+        <v>44</v>
       </c>
       <c r="O70" s="6" t="s">
-        <v>44</v>
-      </c>
-      <c r="P70" s="6" t="s">
         <v>27</v>
       </c>
-      <c r="Q70" s="5"/>
+      <c r="P70" s="5"/>
+      <c r="Q70" s="6" t="s">
+        <v>19</v>
+      </c>
       <c r="R70" s="6" t="s">
         <v>19</v>
       </c>
       <c r="S70" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="T70" s="6" t="s">
-        <v>19</v>
-      </c>
-      <c r="U70" s="6"/>
+      <c r="T70" s="6"/>
     </row>
     <row r="71" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A71" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="B71" s="6" t="s">
-        <v>19</v>
-      </c>
-      <c r="C71" s="6" t="s">
-        <v>19</v>
-      </c>
-      <c r="D71" s="6" t="s">
-        <v>19</v>
-      </c>
-      <c r="E71" s="6" t="s">
+      <c r="B71" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="C71" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="D71" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="E71" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="F71" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="G71" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="I71" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="J71" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="F71" s="6" t="s">
+      <c r="K71" s="6" t="s">
         <v>42</v>
       </c>
-      <c r="G71" s="6" t="s">
+      <c r="L71" s="6" t="s">
         <v>43</v>
       </c>
-      <c r="H71" s="6" t="s">
+      <c r="M71" s="6" t="s">
         <v>43</v>
       </c>
-      <c r="I71" s="6"/>
-      <c r="J71" s="6"/>
-      <c r="K71" s="6"/>
-      <c r="L71" s="6"/>
-      <c r="Q71" s="5"/>
+      <c r="P71" s="5"/>
+      <c r="Q71" s="6" t="s">
+        <v>50</v>
+      </c>
       <c r="R71" s="6" t="s">
-        <v>50</v>
+        <v>37</v>
       </c>
       <c r="S71" s="6" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
       <c r="T71" s="6" t="s">
-        <v>32</v>
-      </c>
-      <c r="U71" s="6" t="s">
         <v>44</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Firm v0.3 - complemento a matrix
</commit_message>
<xml_diff>
--- a/Firmware/v0.3 Stable - Hard 0.0/LCD Layout - Firm v03.xlsx
+++ b/Firmware/v0.3 Stable - Hard 0.0/LCD Layout - Firm v03.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="774" uniqueCount="73">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="779" uniqueCount="73">
   <si>
     <t>01</t>
   </si>
@@ -629,8 +629,8 @@
   <sheetPr codeName="Hoja1"/>
   <dimension ref="A1:AF71"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A43" workbookViewId="0">
-      <selection activeCell="X54" sqref="X54"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -719,53 +719,47 @@
       <c r="A2" s="2" t="s">
         <v>53</v>
       </c>
-      <c r="D2" s="1" t="s">
+      <c r="E2" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="H2" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="I2" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="J2" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="K2" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="M2" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="E2" s="1" t="s">
+      <c r="N2" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="F2" s="1" t="s">
+      <c r="O2" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="G2" s="1" t="s">
+      <c r="P2" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="H2" s="1" t="s">
+      <c r="Q2" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="I2" s="1" t="s">
+      <c r="R2" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="J2" s="1" t="s">
+      <c r="S2" s="1" t="s">
         <v>42</v>
-      </c>
-      <c r="M2" s="1" t="s">
-        <v>58</v>
-      </c>
-      <c r="N2" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="O2" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="P2" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="Q2" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="R2" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="S2" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="T2" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="U2" s="1" t="s">
-        <v>19</v>
       </c>
     </row>
     <row r="3" spans="1:32" x14ac:dyDescent="0.25">
@@ -793,32 +787,35 @@
       <c r="J3" s="1" t="s">
         <v>68</v>
       </c>
+      <c r="L3" s="1" t="s">
+        <v>21</v>
+      </c>
       <c r="M3" s="1" t="s">
-        <v>48</v>
+        <v>35</v>
       </c>
       <c r="N3" s="1" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="O3" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="P3" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="P3" s="1" t="s">
-        <v>33</v>
-      </c>
       <c r="Q3" s="1" t="s">
-        <v>27</v>
+        <v>35</v>
       </c>
       <c r="R3" s="1" t="s">
-        <v>47</v>
+        <v>26</v>
       </c>
       <c r="S3" s="1" t="s">
-        <v>19</v>
+        <v>26</v>
       </c>
       <c r="T3" s="1" t="s">
-        <v>34</v>
+        <v>25</v>
       </c>
       <c r="U3" s="1" t="s">
-        <v>19</v>
+        <v>45</v>
       </c>
     </row>
     <row r="4" spans="1:32" x14ac:dyDescent="0.25">
@@ -826,34 +823,52 @@
         <v>1</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>21</v>
+        <v>58</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>24</v>
+        <v>45</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="F4" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="G4" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="H4" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="I4" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="J4" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="M4" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="N4" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="O4" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="G4" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="H4" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="I4" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="J4" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="K4" s="1" t="s">
-        <v>45</v>
+      <c r="P4" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="R4" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="S4" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="T4" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="U4" s="1" t="s">
+        <v>19</v>
       </c>
     </row>
     <row r="5" spans="1:32" x14ac:dyDescent="0.25">
@@ -1040,7 +1055,7 @@
       <c r="Q8" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="R8" s="1" t="s">
+      <c r="R8" s="5" t="s">
         <v>20</v>
       </c>
       <c r="S8" s="1" t="s">
@@ -3042,6 +3057,22 @@
       </c>
       <c r="H68" s="1" t="s">
         <v>27</v>
+      </c>
+      <c r="P68" s="5"/>
+      <c r="Q68" s="6" t="s">
+        <v>61</v>
+      </c>
+      <c r="R68" s="6" t="s">
+        <v>67</v>
+      </c>
+      <c r="S68" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="T68" s="6" t="s">
+        <v>52</v>
+      </c>
+      <c r="U68" s="1" t="s">
+        <v>44</v>
       </c>
     </row>
     <row r="69" spans="1:21" x14ac:dyDescent="0.25">
@@ -3057,22 +3088,6 @@
       <c r="H69" s="6"/>
       <c r="I69" s="6"/>
       <c r="O69" s="6"/>
-      <c r="P69" s="5"/>
-      <c r="Q69" s="6" t="s">
-        <v>61</v>
-      </c>
-      <c r="R69" s="6" t="s">
-        <v>67</v>
-      </c>
-      <c r="S69" s="6" t="s">
-        <v>35</v>
-      </c>
-      <c r="T69" s="6" t="s">
-        <v>52</v>
-      </c>
-      <c r="U69" s="1" t="s">
-        <v>44</v>
-      </c>
     </row>
     <row r="70" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A70" s="2" t="s">

</xml_diff>

<commit_message>
Firm v0.3 - implementacion en config de control de contraste
</commit_message>
<xml_diff>
--- a/Firmware/v0.3 Stable - Hard 0.0/LCD Layout - Firm v03.xlsx
+++ b/Firmware/v0.3 Stable - Hard 0.0/LCD Layout - Firm v03.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="779" uniqueCount="73">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="791" uniqueCount="73">
   <si>
     <t>01</t>
   </si>
@@ -629,8 +629,8 @@
   <sheetPr codeName="Hoja1"/>
   <dimension ref="A1:AF71"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+    <sheetView tabSelected="1" topLeftCell="A52" workbookViewId="0">
+      <selection activeCell="W71" sqref="W71"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3055,7 +3055,16 @@
       <c r="G68" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="H68" s="1" t="s">
+      <c r="I68" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="J68" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="K68" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="L68" s="1" t="s">
         <v>27</v>
       </c>
       <c r="P68" s="5"/>
@@ -3079,57 +3088,76 @@
       <c r="A69" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B69" s="6"/>
-      <c r="C69" s="6"/>
-      <c r="D69" s="6"/>
-      <c r="E69" s="6"/>
-      <c r="F69" s="6"/>
-      <c r="G69" s="6"/>
-      <c r="H69" s="6"/>
-      <c r="I69" s="6"/>
-      <c r="O69" s="6"/>
+      <c r="E69" s="6" t="s">
+        <v>65</v>
+      </c>
+      <c r="F69" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="G69" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="H69" s="6" t="s">
+        <v>62</v>
+      </c>
+      <c r="J69" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="K69" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="L69" s="6" t="s">
+        <v>64</v>
+      </c>
+      <c r="M69" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="N69" s="6" t="s">
+        <v>44</v>
+      </c>
+      <c r="O69" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="P69" s="5"/>
+      <c r="Q69" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="R69" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="S69" s="6" t="s">
+        <v>19</v>
+      </c>
     </row>
     <row r="70" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A70" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B70" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="C70" s="1" t="s">
+      <c r="G70" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="D70" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="F70" s="6" t="s">
-        <v>65</v>
-      </c>
-      <c r="G70" s="6" t="s">
+      <c r="H70" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="I70" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="J70" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="K70" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="L70" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="H70" s="6" t="s">
-        <v>29</v>
-      </c>
-      <c r="I70" s="6" t="s">
-        <v>62</v>
-      </c>
-      <c r="J70" s="6" t="s">
-        <v>49</v>
-      </c>
-      <c r="K70" s="6" t="s">
-        <v>32</v>
-      </c>
-      <c r="L70" s="6" t="s">
-        <v>64</v>
-      </c>
-      <c r="M70" s="6" t="s">
-        <v>22</v>
-      </c>
-      <c r="N70" s="6" t="s">
+      <c r="M70" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="N70" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="O70" s="6" t="s">
+      <c r="O70" s="1" t="s">
         <v>27</v>
       </c>
       <c r="P70" s="5"/>
@@ -3183,16 +3211,16 @@
       </c>
       <c r="P71" s="5"/>
       <c r="Q71" s="6" t="s">
-        <v>50</v>
+        <v>21</v>
       </c>
       <c r="R71" s="6" t="s">
-        <v>37</v>
+        <v>44</v>
       </c>
       <c r="S71" s="6" t="s">
-        <v>32</v>
+        <v>45</v>
       </c>
       <c r="T71" s="6" t="s">
-        <v>44</v>
+        <v>26</v>
       </c>
     </row>
   </sheetData>

</xml_diff>